<commit_message>
Swapped out temp/humidity sensor
This one is lower power, same functionality, and purchasable
</commit_message>
<xml_diff>
--- a/hardware/rev_c/squall-blees-board_bom.xlsx
+++ b/hardware/rev_c/squall-blees-board_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>Qty</t>
   </si>
@@ -53,27 +53,18 @@
     <t>NEWARK</t>
   </si>
   <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
     <t>CAPACITOR</t>
   </si>
   <si>
     <t>0402_CAP</t>
   </si>
   <si>
-    <t>C4, C5</t>
-  </si>
-  <si>
     <t>0402 Capacitor</t>
   </si>
   <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>C1, C2, C3</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>C6</t>
   </si>
   <si>
-    <t>1kΩ</t>
-  </si>
-  <si>
     <t>RESISTOR0402_RES</t>
   </si>
   <si>
@@ -98,12 +86,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>2kΩ</t>
-  </si>
-  <si>
     <t>R2, R3</t>
   </si>
   <si>
@@ -152,18 +134,12 @@
     <t>68X2585</t>
   </si>
   <si>
-    <t>HTU21DDFN</t>
-  </si>
-  <si>
     <t>DFN</t>
   </si>
   <si>
     <t>U3</t>
   </si>
   <si>
-    <t>This is the HTU21D Temp/Humidity sensor made by BLEES EECS 373.</t>
-  </si>
-  <si>
     <t>LPS331APQFN</t>
   </si>
   <si>
@@ -173,9 +149,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>LPS331AP pressure sensor device designed by BLEES EECS 373</t>
-  </si>
-  <si>
     <t>SQUALL_HEADER</t>
   </si>
   <si>
@@ -188,29 +161,86 @@
     <t>H11617CT-ND</t>
   </si>
   <si>
-    <t>TSL2560DFN</t>
-  </si>
-  <si>
     <t>DFN2</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>TSL2560 light to digital converter, written by BLEES EECS 373.</t>
+    <t>0603 Capacitor</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>0402 Resistor</t>
+  </si>
+  <si>
+    <t>LPS331AP pressure sensor</t>
+  </si>
+  <si>
+    <t>1276-1119-6-ND</t>
+  </si>
+  <si>
+    <t>1276-1442-6-ND</t>
+  </si>
+  <si>
+    <t>160-1647-1-ND</t>
+  </si>
+  <si>
+    <t>RHM1.0KCECT-ND</t>
+  </si>
+  <si>
+    <t>RHM10.0KCDCT-ND</t>
+  </si>
+  <si>
+    <t>52X6707</t>
+  </si>
+  <si>
+    <t>TSL2561DFN</t>
+  </si>
+  <si>
+    <t>TSL2561 light to digital converter</t>
+  </si>
+  <si>
+    <t>TSL2561-FNDKR-ND</t>
+  </si>
+  <si>
+    <t>Si7021</t>
+  </si>
+  <si>
+    <t>Si7021 temperature/humidity sensor</t>
+  </si>
+  <si>
+    <t>336-2542-1-ND</t>
+  </si>
+  <si>
+    <t>ADXL362BCCZ-R2DKR-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,8 +263,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,9 +557,9 @@
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -564,42 +595,48 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
+      <c r="G2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -607,131 +644,143 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>52</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -739,19 +788,22 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -759,19 +811,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -779,39 +834,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -819,5 +857,6 @@
     <sortCondition ref="E2:E13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revisions to BOM for assembler
</commit_message>
<xml_diff>
--- a/hardware/rev_c/squall-blees-board_bom.xlsx
+++ b/hardware/rev_c/squall-blees-board_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>Qty</t>
   </si>
@@ -222,6 +222,30 @@
   </si>
   <si>
     <t>ADXL362BCCZ-R2DKR-ND</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>(s)quall</t>
+  </si>
+  <si>
+    <t>(l)ed box</t>
+  </si>
+  <si>
+    <t>(o)bserver</t>
+  </si>
+  <si>
+    <t>(x) did not populate</t>
+  </si>
+  <si>
+    <t>(b)lees</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -243,12 +267,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,9 +293,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,128 +578,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>47</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -676,165 +717,186 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6">
         <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9">
         <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10">
         <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>59</v>
       </c>
       <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11">
         <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
       </c>
       <c r="C11" t="s">
         <v>62</v>
       </c>
       <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>63</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12">
         <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -843,18 +905,46 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:I13">
-    <sortCondition ref="E2:E13"/>
+  <sortState ref="B2:J13">
+    <sortCondition ref="F2:F13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>